<commit_message>
Update Modern Excel Challenges - Start Here.xlsx
</commit_message>
<xml_diff>
--- a/Excel Series/Modern Excel Challenges - Start Here.xlsx
+++ b/Excel Series/Modern Excel Challenges - Start Here.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://zomalex-my.sharepoint.com/personal/mark_wilcock_zomalex_co_uk/Documents/Courses/Course - Excel Advanced/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\markw\Documents\GitHub\lbag-online\Excel Series\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="365" documentId="11_F25DC773A252ABDACC1048EAE1DC583A5BDE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BC95BB48-56A6-4C0E-852F-F95588345B2B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC2A055D-8A39-4FB7-8D57-54AF637C55E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Split Text" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -463,7 +463,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -499,18 +499,19 @@
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="2"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="2"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Calculation" xfId="2" builtinId="22"/>
@@ -533,10 +534,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1282,9 +1279,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3AF2830-BA34-4632-9D54-EE3F29BC8AC6}">
   <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1340,7 +1335,7 @@
       <c r="C6" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="33" t="s">
+      <c r="D6" s="39" t="s">
         <v>28</v>
       </c>
       <c r="E6" s="27"/>
@@ -1367,8 +1362,8 @@
       <c r="C7" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="33"/>
-      <c r="E7" s="37">
+      <c r="D7" s="39"/>
+      <c r="E7" s="35">
         <v>1.6</v>
       </c>
       <c r="F7" s="30">
@@ -1397,8 +1392,8 @@
         <v>24.489795918367346</v>
       </c>
       <c r="C8" s="31"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="37">
+      <c r="D8" s="39"/>
+      <c r="E8" s="35">
         <v>1.7</v>
       </c>
       <c r="F8" s="30">
@@ -1419,8 +1414,8 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D9" s="33"/>
-      <c r="E9" s="37">
+      <c r="D9" s="39"/>
+      <c r="E9" s="35">
         <v>1.75</v>
       </c>
       <c r="F9" s="30">
@@ -1441,8 +1436,8 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D10" s="33"/>
-      <c r="E10" s="37">
+      <c r="D10" s="39"/>
+      <c r="E10" s="35">
         <v>1.8</v>
       </c>
       <c r="F10" s="30">
@@ -1463,8 +1458,8 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D11" s="33"/>
-      <c r="E11" s="38">
+      <c r="D11" s="39"/>
+      <c r="E11" s="36">
         <v>2</v>
       </c>
       <c r="F11" s="30">
@@ -1502,7 +1497,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D15" s="34" t="s">
+      <c r="D15" s="40" t="s">
         <v>28</v>
       </c>
       <c r="E15" s="7"/>
@@ -1520,8 +1515,8 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D16" s="34"/>
-      <c r="E16" s="35">
+      <c r="D16" s="40"/>
+      <c r="E16" s="33">
         <v>1.6</v>
       </c>
       <c r="F16" s="6"/>
@@ -1530,8 +1525,8 @@
       <c r="I16" s="23"/>
     </row>
     <row r="17" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D17" s="34"/>
-      <c r="E17" s="35">
+      <c r="D17" s="40"/>
+      <c r="E17" s="33">
         <v>1.7</v>
       </c>
       <c r="F17" s="6"/>
@@ -1540,8 +1535,8 @@
       <c r="I17" s="23"/>
     </row>
     <row r="18" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D18" s="34"/>
-      <c r="E18" s="35">
+      <c r="D18" s="40"/>
+      <c r="E18" s="33">
         <v>1.75</v>
       </c>
       <c r="F18" s="6"/>
@@ -1550,8 +1545,8 @@
       <c r="I18" s="23"/>
     </row>
     <row r="19" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D19" s="34"/>
-      <c r="E19" s="35">
+      <c r="D19" s="40"/>
+      <c r="E19" s="33">
         <v>1.8</v>
       </c>
       <c r="F19" s="6"/>
@@ -1560,8 +1555,8 @@
       <c r="I19" s="23"/>
     </row>
     <row r="20" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D20" s="34"/>
-      <c r="E20" s="36">
+      <c r="D20" s="40"/>
+      <c r="E20" s="34">
         <v>2</v>
       </c>
       <c r="F20" s="24"/>
@@ -1580,27 +1575,27 @@
       </c>
     </row>
     <row r="24" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D24" s="34" t="s">
+      <c r="D24" s="40" t="s">
         <v>28</v>
       </c>
       <c r="E24" s="3"/>
-      <c r="F24" s="40" cm="1">
+      <c r="F24" s="38" cm="1">
         <f t="array" ref="F24:I24">_xlfn.SEQUENCE(1,4,70, 10)</f>
         <v>70</v>
       </c>
-      <c r="G24" s="40">
+      <c r="G24" s="38">
         <v>80</v>
       </c>
-      <c r="H24" s="40">
+      <c r="H24" s="38">
         <v>90</v>
       </c>
-      <c r="I24" s="40">
+      <c r="I24" s="38">
         <v>100</v>
       </c>
     </row>
     <row r="25" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D25" s="34"/>
-      <c r="E25" s="40" cm="1">
+      <c r="D25" s="40"/>
+      <c r="E25" s="38" cm="1">
         <f t="array" ref="E25:E29">_xlfn.SEQUENCE(5, 1, 1.6, 0.1)</f>
         <v>1.6</v>
       </c>
@@ -1610,8 +1605,8 @@
       <c r="I25" s="23"/>
     </row>
     <row r="26" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D26" s="34"/>
-      <c r="E26" s="40">
+      <c r="D26" s="40"/>
+      <c r="E26" s="38">
         <v>1.7000000000000002</v>
       </c>
       <c r="F26" s="6"/>
@@ -1620,8 +1615,8 @@
       <c r="I26" s="23"/>
     </row>
     <row r="27" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D27" s="34"/>
-      <c r="E27" s="40">
+      <c r="D27" s="40"/>
+      <c r="E27" s="38">
         <v>1.8000000000000003</v>
       </c>
       <c r="F27" s="6"/>
@@ -1630,8 +1625,8 @@
       <c r="I27" s="23"/>
     </row>
     <row r="28" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D28" s="34"/>
-      <c r="E28" s="40">
+      <c r="D28" s="40"/>
+      <c r="E28" s="38">
         <v>1.9000000000000004</v>
       </c>
       <c r="F28" s="6"/>
@@ -1640,8 +1635,8 @@
       <c r="I28" s="23"/>
     </row>
     <row r="29" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D29" s="34"/>
-      <c r="E29" s="40">
+      <c r="D29" s="40"/>
+      <c r="E29" s="38">
         <v>2.0000000000000004</v>
       </c>
       <c r="F29" s="24"/>
@@ -1667,10 +1662,13 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D33" s="34" t="s">
+      <c r="D33" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="E33" s="7"/>
+      <c r="E33" s="41">
+        <f>B8</f>
+        <v>24.489795918367346</v>
+      </c>
       <c r="F33" s="4">
         <v>60</v>
       </c>
@@ -1685,8 +1683,8 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D34" s="34"/>
-      <c r="E34" s="35">
+      <c r="D34" s="40"/>
+      <c r="E34" s="33">
         <v>1.6</v>
       </c>
       <c r="F34" s="6"/>
@@ -1695,8 +1693,8 @@
       <c r="I34" s="23"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D35" s="34"/>
-      <c r="E35" s="35">
+      <c r="D35" s="40"/>
+      <c r="E35" s="33">
         <v>1.7</v>
       </c>
       <c r="F35" s="6"/>
@@ -1705,8 +1703,8 @@
       <c r="I35" s="23"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D36" s="34"/>
-      <c r="E36" s="35">
+      <c r="D36" s="40"/>
+      <c r="E36" s="33">
         <v>1.75</v>
       </c>
       <c r="F36" s="6"/>
@@ -1715,8 +1713,8 @@
       <c r="I36" s="23"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D37" s="34"/>
-      <c r="E37" s="35">
+      <c r="D37" s="40"/>
+      <c r="E37" s="33">
         <v>1.8</v>
       </c>
       <c r="F37" s="6"/>
@@ -1725,8 +1723,8 @@
       <c r="I37" s="23"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D38" s="34"/>
-      <c r="E38" s="36">
+      <c r="D38" s="40"/>
+      <c r="E38" s="34">
         <v>2</v>
       </c>
       <c r="F38" s="24"/>
@@ -1752,14 +1750,14 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="39" t="s">
+      <c r="A43" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="B43" s="39" cm="1">
+      <c r="B43" s="37" cm="1">
         <f t="array" ref="B43">_xlfn.LAMBDA(_xlpm.weight,_xlpm.height,_xlpm.weight/_xlpm.height^2)(B6,B7)</f>
         <v>24.489795918367346</v>
       </c>
-      <c r="D43" s="34" t="s">
+      <c r="D43" s="40" t="s">
         <v>28</v>
       </c>
       <c r="E43" s="3"/>
@@ -1777,8 +1775,8 @@
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D44" s="34"/>
-      <c r="E44" s="35">
+      <c r="D44" s="40"/>
+      <c r="E44" s="33">
         <v>1.6</v>
       </c>
       <c r="F44" s="6"/>
@@ -1787,8 +1785,8 @@
       <c r="I44" s="23"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D45" s="34"/>
-      <c r="E45" s="35">
+      <c r="D45" s="40"/>
+      <c r="E45" s="33">
         <v>1.7</v>
       </c>
       <c r="F45" s="6"/>
@@ -1797,8 +1795,8 @@
       <c r="I45" s="23"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D46" s="34"/>
-      <c r="E46" s="35">
+      <c r="D46" s="40"/>
+      <c r="E46" s="33">
         <v>1.75</v>
       </c>
       <c r="F46" s="6"/>
@@ -1807,8 +1805,8 @@
       <c r="I46" s="23"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D47" s="34"/>
-      <c r="E47" s="35">
+      <c r="D47" s="40"/>
+      <c r="E47" s="33">
         <v>1.8</v>
       </c>
       <c r="F47" s="6"/>
@@ -1817,8 +1815,8 @@
       <c r="I47" s="23"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D48" s="34"/>
-      <c r="E48" s="36">
+      <c r="D48" s="40"/>
+      <c r="E48" s="34">
         <v>2</v>
       </c>
       <c r="F48" s="24"/>

</xml_diff>